<commit_message>
Tren And Scenar5 (50%)
</commit_message>
<xml_diff>
--- a/Шаблоны/Scenar4.xlsx
+++ b/Шаблоны/Scenar4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="345" yWindow="525" windowWidth="28800" windowHeight="15345" activeTab="2"/>
+    <workbookView xWindow="345" yWindow="525" windowWidth="28800" windowHeight="15345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Отчет" sheetId="1" r:id="rId1"/>
@@ -428,6 +428,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -547,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -564,6 +567,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -871,7 +875,7 @@
       </c>
       <c r="B2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45463</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -961,12 +965,277 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:B85"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B85"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="12"/>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="12"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="12"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="12"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="12"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="12"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="12"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="12"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="12"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="12"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="12"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="12"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="12"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="12"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="12"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="12"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="12"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="12"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="12"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="12"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="12"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="12"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="12"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="12"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="12"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="12"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="12"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="12"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="12"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="12"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="12"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="12"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="12"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="12"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="12"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="12"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="12"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="12"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="12"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="12"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="12"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="12"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="12"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="12"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="12"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="12"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="12"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="12"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="12"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="12"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="12"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="12"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="12"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="12"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="12"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="12"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="12"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="12"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="12"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="12"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="12"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="12"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="12"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -975,7 +1244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>

</xml_diff>